<commit_message>
Post de la S_29
Ajout de l'annexe 3.
exos sur l'ES6.
</commit_message>
<xml_diff>
--- a/S_29/Annexe 3 Programme hebdo de travail 1.xlsx
+++ b/S_29/Annexe 3 Programme hebdo de travail 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\80010-48-01\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB08A8CC-F2E7-4E22-9B1B-ED161C12FAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1375A3C0-DF33-41AC-9CF2-B2DAA069C0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>PROGRAMME HEBDOMADAIRE DE TRAVAIL (des activités réalisées à distance)</t>
   </si>
@@ -109,19 +109,19 @@
     <t>Juillet</t>
   </si>
   <si>
+    <t>ES6</t>
+  </si>
+  <si>
+    <t>DWWM/S_29/ES6</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
     <t>Code Igniter/VillageGreen</t>
   </si>
   <si>
     <t>VillageGreen</t>
-  </si>
-  <si>
-    <t>Github</t>
-  </si>
-  <si>
-    <t>Les failles de sécurité</t>
-  </si>
-  <si>
-    <t>DWWM/S_29/les_failles_de_securite.pdf</t>
   </si>
 </sst>
 </file>
@@ -761,6 +761,87 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -796,87 +877,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1215,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14:L15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1233,14 +1233,14 @@
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -1327,23 +1327,23 @@
       <c r="C7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="68" t="s">
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="70"/>
-      <c r="N7" s="53" t="s">
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="33" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1351,29 +1351,29 @@
       <c r="A8" s="45"/>
       <c r="B8" s="48"/>
       <c r="C8" s="51"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="62" t="s">
+      <c r="D8" s="34"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="63"/>
-      <c r="L8" s="64" t="s">
+      <c r="K8" s="36"/>
+      <c r="L8" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="66" t="s">
+      <c r="M8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="54"/>
+      <c r="N8" s="34"/>
     </row>
     <row r="9" spans="1:14" ht="90">
       <c r="A9" s="46"/>
       <c r="B9" s="49"/>
       <c r="C9" s="52"/>
-      <c r="D9" s="54"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="10" t="s">
         <v>16</v>
       </c>
@@ -1395,15 +1395,15 @@
       <c r="K9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="65"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="54"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="34"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="65">
         <v>29</v>
       </c>
       <c r="C10" s="19">
@@ -1417,7 +1417,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="26">
-        <v>44389</v>
+        <v>44396</v>
       </c>
       <c r="J10" s="20"/>
       <c r="K10" s="11" t="s">
@@ -1430,24 +1430,24 @@
       <c r="N10" s="19"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="42"/>
-      <c r="B11" s="39"/>
+      <c r="A11" s="69"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="19">
         <v>13</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="26">
-        <v>44390</v>
+        <v>44397</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L11" s="11" t="s">
         <v>26</v>
@@ -1456,24 +1456,24 @@
       <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="42"/>
-      <c r="B12" s="39"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="19">
         <v>14</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="26">
-        <v>44391</v>
+        <v>44398</v>
       </c>
       <c r="J12" s="14"/>
       <c r="K12" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L12" s="11" t="s">
         <v>26</v>
@@ -1482,24 +1482,24 @@
       <c r="N12" s="12"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="42"/>
-      <c r="B13" s="39"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="19">
         <v>15</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="26">
-        <v>44392</v>
+        <v>44399</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L13" s="11" t="s">
         <v>26</v>
@@ -1508,24 +1508,24 @@
       <c r="N13" s="12"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="42"/>
-      <c r="B14" s="39"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="19">
         <v>16</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="26">
-        <v>44393</v>
+        <v>44400</v>
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L14" s="11" t="s">
         <v>26</v>
@@ -1534,34 +1534,24 @@
       <c r="N14" s="12"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="42"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="19">
-        <v>16</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>27</v>
-      </c>
+      <c r="A15" s="69"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="26">
-        <v>44393</v>
-      </c>
+      <c r="I15" s="26"/>
       <c r="J15" s="14"/>
-      <c r="K15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="15"/>
       <c r="N15" s="12"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="42"/>
-      <c r="B16" s="39"/>
+      <c r="A16" s="69"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="12"/>
       <c r="D16" s="19"/>
       <c r="E16" s="11"/>
@@ -1576,8 +1566,8 @@
       <c r="N16" s="12"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="42"/>
-      <c r="B17" s="39"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="27"/>
       <c r="D17" s="19"/>
       <c r="E17" s="11"/>
@@ -1592,8 +1582,8 @@
       <c r="N17" s="12"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="42"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="69"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="27"/>
       <c r="D18" s="19"/>
       <c r="E18" s="11"/>
@@ -1608,8 +1598,8 @@
       <c r="N18" s="12"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="42"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="12"/>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
@@ -1624,8 +1614,8 @@
       <c r="N19" s="12"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="42"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="12"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
@@ -1640,8 +1630,8 @@
       <c r="N20" s="12"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="42"/>
-      <c r="B21" s="39"/>
+      <c r="A21" s="69"/>
+      <c r="B21" s="66"/>
       <c r="C21" s="12"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
@@ -1656,8 +1646,8 @@
       <c r="N21" s="12"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="42"/>
-      <c r="B22" s="39"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="12"/>
       <c r="D22" s="29"/>
       <c r="E22" s="19"/>
@@ -1672,8 +1662,8 @@
       <c r="N22" s="12"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="42"/>
-      <c r="B23" s="39"/>
+      <c r="A23" s="69"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="12"/>
       <c r="D23" s="29"/>
       <c r="E23" s="19"/>
@@ -1688,8 +1678,8 @@
       <c r="N23" s="12"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="42"/>
-      <c r="B24" s="39"/>
+      <c r="A24" s="69"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="12"/>
       <c r="D24" s="29"/>
       <c r="E24" s="19"/>
@@ -1704,8 +1694,8 @@
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="42"/>
-      <c r="B25" s="39"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="14"/>
@@ -1720,8 +1710,8 @@
       <c r="N25" s="12"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="42"/>
-      <c r="B26" s="39"/>
+      <c r="A26" s="69"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="14"/>
@@ -1736,8 +1726,8 @@
       <c r="N26" s="12"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="42"/>
-      <c r="B27" s="39"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="66"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="14"/>
@@ -1752,8 +1742,8 @@
       <c r="N27" s="12"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="42"/>
-      <c r="B28" s="39"/>
+      <c r="A28" s="69"/>
+      <c r="B28" s="66"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="14"/>
@@ -1768,8 +1758,8 @@
       <c r="N28" s="12"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="42"/>
-      <c r="B29" s="39"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="66"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="14"/>
@@ -1784,8 +1774,8 @@
       <c r="N29" s="12"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="42"/>
-      <c r="B30" s="39"/>
+      <c r="A30" s="69"/>
+      <c r="B30" s="66"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="14"/>
@@ -1800,8 +1790,8 @@
       <c r="N30" s="12"/>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="42"/>
-      <c r="B31" s="39"/>
+      <c r="A31" s="69"/>
+      <c r="B31" s="66"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="14"/>
@@ -1816,8 +1806,8 @@
       <c r="N31" s="12"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="42"/>
-      <c r="B32" s="39"/>
+      <c r="A32" s="69"/>
+      <c r="B32" s="66"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="14"/>
@@ -1832,8 +1822,8 @@
       <c r="N32" s="12"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="43"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="70"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
@@ -1849,8 +1839,8 @@
     </row>
     <row r="34" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="35" spans="1:14">
-      <c r="A35" s="32"/>
-      <c r="B35" s="35"/>
+      <c r="A35" s="59"/>
+      <c r="B35" s="62"/>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
       <c r="E35" s="20"/>
@@ -1865,8 +1855,8 @@
       <c r="N35" s="19"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="33"/>
-      <c r="B36" s="36"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="63"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="14"/>
@@ -1881,8 +1871,8 @@
       <c r="N36" s="12"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="33"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="63"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="14"/>
@@ -1897,8 +1887,8 @@
       <c r="N37" s="12"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="33"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="60"/>
+      <c r="B38" s="63"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="14"/>
@@ -1913,8 +1903,8 @@
       <c r="N38" s="12"/>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="33"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="60"/>
+      <c r="B39" s="63"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="14"/>
@@ -1929,8 +1919,8 @@
       <c r="N39" s="12"/>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="33"/>
-      <c r="B40" s="36"/>
+      <c r="A40" s="60"/>
+      <c r="B40" s="63"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="14"/>
@@ -1945,8 +1935,8 @@
       <c r="N40" s="12"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="33"/>
-      <c r="B41" s="36"/>
+      <c r="A41" s="60"/>
+      <c r="B41" s="63"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="14"/>
@@ -1961,8 +1951,8 @@
       <c r="N41" s="12"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="33"/>
-      <c r="B42" s="36"/>
+      <c r="A42" s="60"/>
+      <c r="B42" s="63"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="14"/>
@@ -1977,8 +1967,8 @@
       <c r="N42" s="12"/>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="33"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="60"/>
+      <c r="B43" s="63"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
       <c r="E43" s="14"/>
@@ -1993,8 +1983,8 @@
       <c r="N43" s="12"/>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="33"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="60"/>
+      <c r="B44" s="63"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="14"/>
@@ -2009,8 +1999,8 @@
       <c r="N44" s="12"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="33"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="60"/>
+      <c r="B45" s="63"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
       <c r="E45" s="14"/>
@@ -2025,8 +2015,8 @@
       <c r="N45" s="12"/>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="33"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="60"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="14"/>
@@ -2041,8 +2031,8 @@
       <c r="N46" s="12"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="33"/>
-      <c r="B47" s="36"/>
+      <c r="A47" s="60"/>
+      <c r="B47" s="63"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="14"/>
@@ -2057,8 +2047,8 @@
       <c r="N47" s="12"/>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="33"/>
-      <c r="B48" s="36"/>
+      <c r="A48" s="60"/>
+      <c r="B48" s="63"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="14"/>
@@ -2073,8 +2063,8 @@
       <c r="N48" s="12"/>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="33"/>
-      <c r="B49" s="36"/>
+      <c r="A49" s="60"/>
+      <c r="B49" s="63"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="14"/>
@@ -2089,8 +2079,8 @@
       <c r="N49" s="12"/>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="33"/>
-      <c r="B50" s="36"/>
+      <c r="A50" s="60"/>
+      <c r="B50" s="63"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="14"/>
@@ -2105,8 +2095,8 @@
       <c r="N50" s="12"/>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="33"/>
-      <c r="B51" s="36"/>
+      <c r="A51" s="60"/>
+      <c r="B51" s="63"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
       <c r="E51" s="14"/>
@@ -2121,8 +2111,8 @@
       <c r="N51" s="12"/>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="33"/>
-      <c r="B52" s="36"/>
+      <c r="A52" s="60"/>
+      <c r="B52" s="63"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="14"/>
@@ -2137,8 +2127,8 @@
       <c r="N52" s="12"/>
     </row>
     <row r="53" spans="1:14">
-      <c r="A53" s="33"/>
-      <c r="B53" s="36"/>
+      <c r="A53" s="60"/>
+      <c r="B53" s="63"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="14"/>
@@ -2153,8 +2143,8 @@
       <c r="N53" s="12"/>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="33"/>
-      <c r="B54" s="36"/>
+      <c r="A54" s="60"/>
+      <c r="B54" s="63"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="14"/>
@@ -2169,8 +2159,8 @@
       <c r="N54" s="12"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="33"/>
-      <c r="B55" s="36"/>
+      <c r="A55" s="60"/>
+      <c r="B55" s="63"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="14"/>
@@ -2185,8 +2175,8 @@
       <c r="N55" s="12"/>
     </row>
     <row r="56" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A56" s="34"/>
-      <c r="B56" s="37"/>
+      <c r="A56" s="61"/>
+      <c r="B56" s="64"/>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
       <c r="E56" s="16"/>
@@ -2202,8 +2192,8 @@
     </row>
     <row r="57" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="58" spans="1:14">
-      <c r="A58" s="32"/>
-      <c r="B58" s="35"/>
+      <c r="A58" s="59"/>
+      <c r="B58" s="62"/>
       <c r="C58" s="19"/>
       <c r="D58" s="19"/>
       <c r="E58" s="20"/>
@@ -2218,8 +2208,8 @@
       <c r="N58" s="19"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="33"/>
-      <c r="B59" s="36"/>
+      <c r="A59" s="60"/>
+      <c r="B59" s="63"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="14"/>
@@ -2234,8 +2224,8 @@
       <c r="N59" s="12"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="33"/>
-      <c r="B60" s="36"/>
+      <c r="A60" s="60"/>
+      <c r="B60" s="63"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="14"/>
@@ -2250,8 +2240,8 @@
       <c r="N60" s="12"/>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="33"/>
-      <c r="B61" s="36"/>
+      <c r="A61" s="60"/>
+      <c r="B61" s="63"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
       <c r="E61" s="14"/>
@@ -2266,8 +2256,8 @@
       <c r="N61" s="12"/>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="33"/>
-      <c r="B62" s="36"/>
+      <c r="A62" s="60"/>
+      <c r="B62" s="63"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
       <c r="E62" s="14"/>
@@ -2282,8 +2272,8 @@
       <c r="N62" s="12"/>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="33"/>
-      <c r="B63" s="36"/>
+      <c r="A63" s="60"/>
+      <c r="B63" s="63"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="14"/>
@@ -2298,8 +2288,8 @@
       <c r="N63" s="12"/>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="33"/>
-      <c r="B64" s="36"/>
+      <c r="A64" s="60"/>
+      <c r="B64" s="63"/>
       <c r="C64" s="12"/>
       <c r="D64" s="12"/>
       <c r="E64" s="14"/>
@@ -2314,8 +2304,8 @@
       <c r="N64" s="12"/>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="33"/>
-      <c r="B65" s="36"/>
+      <c r="A65" s="60"/>
+      <c r="B65" s="63"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
       <c r="E65" s="14"/>
@@ -2330,8 +2320,8 @@
       <c r="N65" s="12"/>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="33"/>
-      <c r="B66" s="36"/>
+      <c r="A66" s="60"/>
+      <c r="B66" s="63"/>
       <c r="C66" s="12"/>
       <c r="D66" s="12"/>
       <c r="E66" s="14"/>
@@ -2346,8 +2336,8 @@
       <c r="N66" s="12"/>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="33"/>
-      <c r="B67" s="36"/>
+      <c r="A67" s="60"/>
+      <c r="B67" s="63"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
       <c r="E67" s="14"/>
@@ -2362,8 +2352,8 @@
       <c r="N67" s="12"/>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="33"/>
-      <c r="B68" s="36"/>
+      <c r="A68" s="60"/>
+      <c r="B68" s="63"/>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
       <c r="E68" s="14"/>
@@ -2378,8 +2368,8 @@
       <c r="N68" s="12"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="33"/>
-      <c r="B69" s="36"/>
+      <c r="A69" s="60"/>
+      <c r="B69" s="63"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
       <c r="E69" s="14"/>
@@ -2394,8 +2384,8 @@
       <c r="N69" s="12"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="33"/>
-      <c r="B70" s="36"/>
+      <c r="A70" s="60"/>
+      <c r="B70" s="63"/>
       <c r="C70" s="12"/>
       <c r="D70" s="12"/>
       <c r="E70" s="14"/>
@@ -2410,8 +2400,8 @@
       <c r="N70" s="12"/>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="33"/>
-      <c r="B71" s="36"/>
+      <c r="A71" s="60"/>
+      <c r="B71" s="63"/>
       <c r="C71" s="12"/>
       <c r="D71" s="12"/>
       <c r="E71" s="14"/>
@@ -2426,8 +2416,8 @@
       <c r="N71" s="12"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="33"/>
-      <c r="B72" s="36"/>
+      <c r="A72" s="60"/>
+      <c r="B72" s="63"/>
       <c r="C72" s="12"/>
       <c r="D72" s="12"/>
       <c r="E72" s="14"/>
@@ -2442,8 +2432,8 @@
       <c r="N72" s="12"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="33"/>
-      <c r="B73" s="36"/>
+      <c r="A73" s="60"/>
+      <c r="B73" s="63"/>
       <c r="C73" s="12"/>
       <c r="D73" s="12"/>
       <c r="E73" s="14"/>
@@ -2458,8 +2448,8 @@
       <c r="N73" s="12"/>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="33"/>
-      <c r="B74" s="36"/>
+      <c r="A74" s="60"/>
+      <c r="B74" s="63"/>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="14"/>
@@ -2474,8 +2464,8 @@
       <c r="N74" s="12"/>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="33"/>
-      <c r="B75" s="36"/>
+      <c r="A75" s="60"/>
+      <c r="B75" s="63"/>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
       <c r="E75" s="14"/>
@@ -2490,8 +2480,8 @@
       <c r="N75" s="12"/>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="33"/>
-      <c r="B76" s="36"/>
+      <c r="A76" s="60"/>
+      <c r="B76" s="63"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
       <c r="E76" s="14"/>
@@ -2506,8 +2496,8 @@
       <c r="N76" s="12"/>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="33"/>
-      <c r="B77" s="36"/>
+      <c r="A77" s="60"/>
+      <c r="B77" s="63"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
       <c r="E77" s="14"/>
@@ -2522,8 +2512,8 @@
       <c r="N77" s="12"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="33"/>
-      <c r="B78" s="36"/>
+      <c r="A78" s="60"/>
+      <c r="B78" s="63"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
       <c r="E78" s="14"/>
@@ -2538,8 +2528,8 @@
       <c r="N78" s="12"/>
     </row>
     <row r="79" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A79" s="34"/>
-      <c r="B79" s="37"/>
+      <c r="A79" s="61"/>
+      <c r="B79" s="64"/>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
       <c r="E79" s="16"/>
@@ -2555,23 +2545,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A58:A79"/>
+    <mergeCell ref="B58:B79"/>
+    <mergeCell ref="B10:B33"/>
+    <mergeCell ref="A10:A33"/>
+    <mergeCell ref="A35:A56"/>
+    <mergeCell ref="B35:B56"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:I8"/>
     <mergeCell ref="F2:K2"/>
     <mergeCell ref="N7:N9"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="J7:M7"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:I8"/>
-    <mergeCell ref="A58:A79"/>
-    <mergeCell ref="B58:B79"/>
-    <mergeCell ref="B10:B33"/>
-    <mergeCell ref="A10:A33"/>
-    <mergeCell ref="A35:A56"/>
-    <mergeCell ref="B35:B56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2579,6 +2569,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C44A67B3B57D954BAE559FE843CA0F3B" ma:contentTypeVersion="0" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="fa0ae4ffadfaf6fcc6c2c602ec821808">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3d6ca9f312fcd1c0ab10337cdbdb729">
     <xsd:element name="properties">
@@ -2692,12 +2688,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2708,11 +2698,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E1FD49D-F402-44CA-B239-B9C3B2CCC1EF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80C1555C-3F52-4E61-B55F-20AC6C94620E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80C1555C-3F52-4E61-B55F-20AC6C94620E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E1FD49D-F402-44CA-B239-B9C3B2CCC1EF}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>